<commit_message>
create Annual Sales column and calculated the values
</commit_message>
<xml_diff>
--- a/Discount-Variety-Store-433-Monthly-Sales.xlsx
+++ b/Discount-Variety-Store-433-Monthly-Sales.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Common-Calculation-Fomulas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B1B6B0-0E75-45F5-A9CF-0FA231CDCBC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Discount-Variety-Store-433-Mont" sheetId="1" r:id="rId4"/>
+    <sheet name="Discount-Variety-Store-433-Mont" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Monthly sales</t>
   </si>
@@ -50,23 +59,27 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Annual Sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -77,39 +90,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -299,20 +318,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -352,418 +376,461 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="B2" s="2">
-        <v>47563.0</v>
+        <v>47563</v>
       </c>
       <c r="C2" s="2">
-        <v>49078.0</v>
+        <v>49078</v>
       </c>
       <c r="D2" s="2">
-        <v>51324.0</v>
+        <v>51324</v>
       </c>
       <c r="E2" s="2">
-        <v>55678.0</v>
+        <v>55678</v>
       </c>
       <c r="F2" s="2">
-        <v>54687.0</v>
+        <v>54687</v>
       </c>
       <c r="G2" s="2">
-        <v>72013.0</v>
+        <v>72013</v>
       </c>
       <c r="H2" s="2">
-        <v>80443.0</v>
+        <v>80443</v>
       </c>
       <c r="I2" s="2">
-        <v>86785.0</v>
+        <v>86785</v>
       </c>
       <c r="J2" s="2">
-        <v>90876.0</v>
+        <v>90876</v>
       </c>
       <c r="K2" s="2">
-        <v>67712.0</v>
+        <v>67712</v>
       </c>
       <c r="L2" s="2">
-        <v>70048.0</v>
+        <v>70048</v>
       </c>
       <c r="M2" s="2">
-        <v>145378.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>145378</v>
+      </c>
+      <c r="N2" s="3">
+        <f>SUM(B2:M2)</f>
+        <v>871585</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2012.0</v>
+        <v>2012</v>
       </c>
       <c r="B3" s="2">
-        <v>39575.0</v>
+        <v>39575</v>
       </c>
       <c r="C3" s="2">
-        <v>50384.0</v>
+        <v>50384</v>
       </c>
       <c r="D3" s="2">
-        <v>56827.0</v>
+        <v>56827</v>
       </c>
       <c r="E3" s="2">
-        <v>60401.0</v>
+        <v>60401</v>
       </c>
       <c r="F3" s="2">
-        <v>59802.0</v>
+        <v>59802</v>
       </c>
       <c r="G3" s="2">
-        <v>84023.0</v>
+        <v>84023</v>
       </c>
       <c r="H3" s="2">
-        <v>59733.0</v>
+        <v>59733</v>
       </c>
       <c r="I3" s="2">
-        <v>86568.0</v>
+        <v>86568</v>
       </c>
       <c r="J3" s="2">
-        <v>90986.0</v>
+        <v>90986</v>
       </c>
       <c r="K3" s="2">
-        <v>68145.0</v>
+        <v>68145</v>
       </c>
       <c r="L3" s="2">
-        <v>81811.0</v>
+        <v>81811</v>
       </c>
       <c r="M3" s="2">
-        <v>199468.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>199468</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" ref="N3:N11" si="0">SUM(B3:M3)</f>
+        <v>937723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="B4" s="2">
-        <v>56591.0</v>
+        <v>56591</v>
       </c>
       <c r="C4" s="2">
-        <v>50319.0</v>
+        <v>50319</v>
       </c>
       <c r="D4" s="2">
-        <v>51627.0</v>
+        <v>51627</v>
       </c>
       <c r="E4" s="2">
-        <v>53040.0</v>
+        <v>53040</v>
       </c>
       <c r="F4" s="2">
-        <v>63607.0</v>
+        <v>63607</v>
       </c>
       <c r="G4" s="2">
-        <v>84145.0</v>
+        <v>84145</v>
       </c>
       <c r="H4" s="2">
-        <v>72511.0</v>
+        <v>72511</v>
       </c>
       <c r="I4" s="2">
-        <v>91004.0</v>
+        <v>91004</v>
       </c>
       <c r="J4" s="2">
-        <v>95838.0</v>
+        <v>95838</v>
       </c>
       <c r="K4" s="2">
-        <v>70003.0</v>
+        <v>70003</v>
       </c>
       <c r="L4" s="2">
-        <v>79809.0</v>
+        <v>79809</v>
       </c>
       <c r="M4" s="2">
-        <v>155736.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>155736</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="0"/>
+        <v>924230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="B5" s="2">
-        <v>39113.0</v>
+        <v>39113</v>
       </c>
       <c r="C5" s="2">
-        <v>40107.0</v>
+        <v>40107</v>
       </c>
       <c r="D5" s="2">
-        <v>52332.0</v>
+        <v>52332</v>
       </c>
       <c r="E5" s="2">
-        <v>63681.0</v>
+        <v>63681</v>
       </c>
       <c r="F5" s="2">
-        <v>54788.0</v>
+        <v>54788</v>
       </c>
       <c r="G5" s="2">
-        <v>69505.0</v>
+        <v>69505</v>
       </c>
       <c r="H5" s="2">
-        <v>69789.0</v>
+        <v>69789</v>
       </c>
       <c r="I5" s="2">
-        <v>80030.0</v>
+        <v>80030</v>
       </c>
       <c r="J5" s="2">
-        <v>96448.0</v>
+        <v>96448</v>
       </c>
       <c r="K5" s="2">
-        <v>70317.0</v>
+        <v>70317</v>
       </c>
       <c r="L5" s="2">
-        <v>74153.0</v>
+        <v>74153</v>
       </c>
       <c r="M5" s="2">
-        <v>160152.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>160152</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="0"/>
+        <v>870415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="B6" s="2">
-        <v>41666.0</v>
+        <v>41666</v>
       </c>
       <c r="C6" s="2">
-        <v>53993.0</v>
+        <v>53993</v>
       </c>
       <c r="D6" s="2">
-        <v>43428.0</v>
+        <v>43428</v>
       </c>
       <c r="E6" s="2">
-        <v>64898.0</v>
+        <v>64898</v>
       </c>
       <c r="F6" s="2">
-        <v>58070.0</v>
+        <v>58070</v>
       </c>
       <c r="G6" s="2">
-        <v>77845.0</v>
+        <v>77845</v>
       </c>
       <c r="H6" s="2">
-        <v>79131.0</v>
+        <v>79131</v>
       </c>
       <c r="I6" s="2">
-        <v>83993.0</v>
+        <v>83993</v>
       </c>
       <c r="J6" s="2">
-        <v>93311.0</v>
+        <v>93311</v>
       </c>
       <c r="K6" s="2">
-        <v>67773.0</v>
+        <v>67773</v>
       </c>
       <c r="L6" s="2">
-        <v>71925.0</v>
+        <v>71925</v>
       </c>
       <c r="M6" s="2">
-        <v>159231.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>159231</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="0"/>
+        <v>895264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="B7" s="2">
-        <v>38405.0</v>
+        <v>38405</v>
       </c>
       <c r="C7" s="2">
-        <v>46658.0</v>
+        <v>46658</v>
       </c>
       <c r="D7" s="2">
-        <v>40267.0</v>
+        <v>40267</v>
       </c>
       <c r="E7" s="2">
-        <v>53313.0</v>
+        <v>53313</v>
       </c>
       <c r="F7" s="2">
-        <v>57532.0</v>
+        <v>57532</v>
       </c>
       <c r="G7" s="2">
-        <v>78583.0</v>
+        <v>78583</v>
       </c>
       <c r="H7" s="2">
-        <v>70271.0</v>
+        <v>70271</v>
       </c>
       <c r="I7" s="2">
-        <v>88744.0</v>
+        <v>88744</v>
       </c>
       <c r="J7" s="2">
-        <v>95468.0</v>
+        <v>95468</v>
       </c>
       <c r="K7" s="2">
-        <v>66886.0</v>
+        <v>66886</v>
       </c>
       <c r="L7" s="2">
-        <v>82020.0</v>
+        <v>82020</v>
       </c>
       <c r="M7" s="2">
-        <v>162724.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>162724</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="0"/>
+        <v>880871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="B8" s="2">
-        <v>41756.0</v>
+        <v>41756</v>
       </c>
       <c r="C8" s="2">
-        <v>41311.0</v>
+        <v>41311</v>
       </c>
       <c r="D8" s="2">
-        <v>50981.0</v>
+        <v>50981</v>
       </c>
       <c r="E8" s="2">
-        <v>62467.0</v>
+        <v>62467</v>
       </c>
       <c r="F8" s="2">
-        <v>54526.0</v>
+        <v>54526</v>
       </c>
       <c r="G8" s="2">
-        <v>84282.0</v>
+        <v>84282</v>
       </c>
       <c r="H8" s="2">
-        <v>73403.0</v>
+        <v>73403</v>
       </c>
       <c r="I8" s="2">
-        <v>82530.0</v>
+        <v>82530</v>
       </c>
       <c r="J8" s="2">
-        <v>92958.0</v>
+        <v>92958</v>
       </c>
       <c r="K8" s="2">
-        <v>67167.0</v>
+        <v>67167</v>
       </c>
       <c r="L8" s="2">
-        <v>75553.0</v>
+        <v>75553</v>
       </c>
       <c r="M8" s="2">
-        <v>161102.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>161102</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="0"/>
+        <v>888036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="B9" s="2">
-        <v>56061.0</v>
+        <v>56061</v>
       </c>
       <c r="C9" s="2">
-        <v>40703.0</v>
+        <v>40703</v>
       </c>
       <c r="D9" s="2">
-        <v>47350.0</v>
+        <v>47350</v>
       </c>
       <c r="E9" s="2">
-        <v>56515.0</v>
+        <v>56515</v>
       </c>
       <c r="F9" s="2">
-        <v>60270.0</v>
+        <v>60270</v>
       </c>
       <c r="G9" s="2">
-        <v>75195.0</v>
+        <v>75195</v>
       </c>
       <c r="H9" s="2">
-        <v>70765.0</v>
+        <v>70765</v>
       </c>
       <c r="I9" s="2">
-        <v>89011.0</v>
+        <v>89011</v>
       </c>
       <c r="J9" s="2">
-        <v>91707.0</v>
+        <v>91707</v>
       </c>
       <c r="K9" s="2">
-        <v>73375.0</v>
+        <v>73375</v>
       </c>
       <c r="L9" s="2">
-        <v>77740.0</v>
+        <v>77740</v>
       </c>
       <c r="M9" s="2">
-        <v>182880.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>182880</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="0"/>
+        <v>921572</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2019.0</v>
+        <v>2019</v>
       </c>
       <c r="B10" s="2">
-        <v>57355.0</v>
+        <v>57355</v>
       </c>
       <c r="C10" s="2">
-        <v>46703.0</v>
+        <v>46703</v>
       </c>
       <c r="D10" s="2">
-        <v>44234.0</v>
+        <v>44234</v>
       </c>
       <c r="E10" s="2">
-        <v>57172.0</v>
+        <v>57172</v>
       </c>
       <c r="F10" s="2">
-        <v>63455.0</v>
+        <v>63455</v>
       </c>
       <c r="G10" s="2">
-        <v>72180.0</v>
+        <v>72180</v>
       </c>
       <c r="H10" s="2">
-        <v>82110.0</v>
+        <v>82110</v>
       </c>
       <c r="I10" s="2">
-        <v>90201.0</v>
+        <v>90201</v>
       </c>
       <c r="J10" s="2">
-        <v>90814.0</v>
+        <v>90814</v>
       </c>
       <c r="K10" s="2">
-        <v>69444.0</v>
+        <v>69444</v>
       </c>
       <c r="L10" s="2">
-        <v>73301.0</v>
+        <v>73301</v>
       </c>
       <c r="M10" s="2">
-        <v>192224.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>192224</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="0"/>
+        <v>939193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>2020.0</v>
+        <v>2020</v>
       </c>
       <c r="B11" s="2">
-        <v>42234.0</v>
+        <v>42234</v>
       </c>
       <c r="C11" s="2">
-        <v>54050.0</v>
+        <v>54050</v>
       </c>
       <c r="D11" s="2">
-        <v>42377.0</v>
+        <v>42377</v>
       </c>
       <c r="E11" s="2">
-        <v>61252.0</v>
+        <v>61252</v>
       </c>
       <c r="F11" s="2">
-        <v>55787.0</v>
+        <v>55787</v>
       </c>
       <c r="G11" s="2">
-        <v>78382.0</v>
+        <v>78382</v>
       </c>
       <c r="H11" s="2">
-        <v>88438.0</v>
+        <v>88438</v>
       </c>
       <c r="I11" s="2">
-        <v>89150.0</v>
+        <v>89150</v>
       </c>
       <c r="J11" s="2">
-        <v>95810.0</v>
+        <v>95810</v>
       </c>
       <c r="K11" s="2">
-        <v>70843.0</v>
+        <v>70843</v>
       </c>
       <c r="L11" s="2">
-        <v>75393.0</v>
+        <v>75393</v>
       </c>
       <c r="M11" s="2">
-        <v>137534.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>137534</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="0"/>
+        <v>891250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -777,13 +844,13 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add column 'Growth from Previous Year'
</commit_message>
<xml_diff>
--- a/Discount-Variety-Store-433-Monthly-Sales.xlsx
+++ b/Discount-Variety-Store-433-Monthly-Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Common-Calculation-Fomulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B1B6B0-0E75-45F5-A9CF-0FA231CDCBC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7DE299-B3C9-4FBA-B9C8-9D28D7CF4473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Monthly sales</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Annual Sales</t>
+  </si>
+  <si>
+    <t>Growth from Previous Year</t>
   </si>
 </sst>
 </file>
@@ -328,15 +331,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N11"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -379,8 +385,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
@@ -425,7 +434,7 @@
         <v>871585</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
@@ -469,8 +478,12 @@
         <f t="shared" ref="N3:N11" si="0">SUM(B3:M3)</f>
         <v>937723</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="3">
+        <f>N3-N2</f>
+        <v>66138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2013</v>
       </c>
@@ -514,8 +527,12 @@
         <f t="shared" si="0"/>
         <v>924230</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="3">
+        <f t="shared" ref="O4:O11" si="1">N4-N3</f>
+        <v>-13493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2014</v>
       </c>
@@ -559,8 +576,12 @@
         <f t="shared" si="0"/>
         <v>870415</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="3">
+        <f t="shared" si="1"/>
+        <v>-53815</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -604,8 +625,12 @@
         <f t="shared" si="0"/>
         <v>895264</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="3">
+        <f t="shared" si="1"/>
+        <v>24849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
@@ -649,8 +674,12 @@
         <f t="shared" si="0"/>
         <v>880871</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="3">
+        <f t="shared" si="1"/>
+        <v>-14393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
@@ -694,8 +723,12 @@
         <f t="shared" si="0"/>
         <v>888036</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="3">
+        <f t="shared" si="1"/>
+        <v>7165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
@@ -739,8 +772,12 @@
         <f t="shared" si="0"/>
         <v>921572</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="3">
+        <f t="shared" si="1"/>
+        <v>33536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
@@ -784,8 +821,12 @@
         <f t="shared" si="0"/>
         <v>939193</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="3">
+        <f t="shared" si="1"/>
+        <v>17621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2020</v>
       </c>
@@ -829,8 +870,12 @@
         <f t="shared" si="0"/>
         <v>891250</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="3">
+        <f t="shared" si="1"/>
+        <v>-47943</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -844,10 +889,10 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apply conditional formatting to the cells with the Average Sales by month
</commit_message>
<xml_diff>
--- a/Discount-Variety-Store-433-Monthly-Sales.xlsx
+++ b/Discount-Variety-Store-433-Monthly-Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Common-Calculation-Fomulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7DE299-B3C9-4FBA-B9C8-9D28D7CF4473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1347C6F-FEE1-47CD-9F91-7E43E5890C65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Monthly sales</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Growth from Previous Year</t>
+  </si>
+  <si>
+    <t>%growth</t>
+  </si>
+  <si>
+    <t>Average by month</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -85,6 +91,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,17 +124,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,18 +354,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,8 +413,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2011</v>
       </c>
@@ -434,7 +462,7 @@
         <v>871585</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2012</v>
       </c>
@@ -482,8 +510,12 @@
         <f>N3-N2</f>
         <v>66138</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="4">
+        <f>O3/N2</f>
+        <v>7.5882444053075718E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2013</v>
       </c>
@@ -531,8 +563,12 @@
         <f t="shared" ref="O4:O11" si="1">N4-N3</f>
         <v>-13493</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="4">
+        <f t="shared" ref="P4:P11" si="2">O4/N3</f>
+        <v>-1.4389110643548255E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2014</v>
       </c>
@@ -580,8 +616,12 @@
         <f t="shared" si="1"/>
         <v>-53815</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="4">
+        <f t="shared" si="2"/>
+        <v>-5.8226848295337738E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2015</v>
       </c>
@@ -629,8 +669,12 @@
         <f t="shared" si="1"/>
         <v>24849</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="4">
+        <f t="shared" si="2"/>
+        <v>2.8548451026234611E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
@@ -678,8 +722,12 @@
         <f t="shared" si="1"/>
         <v>-14393</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.6076822032383743E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2017</v>
       </c>
@@ -727,8 +775,12 @@
         <f t="shared" si="1"/>
         <v>7165</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="4">
+        <f t="shared" si="2"/>
+        <v>8.1339946484786079E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
@@ -776,8 +828,12 @@
         <f t="shared" si="1"/>
         <v>33536</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="4">
+        <f t="shared" si="2"/>
+        <v>3.776423478327455E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2019</v>
       </c>
@@ -825,8 +881,12 @@
         <f t="shared" si="1"/>
         <v>17621</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="4">
+        <f t="shared" si="2"/>
+        <v>1.9120589601246567E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2020</v>
       </c>
@@ -874,28 +934,90 @@
         <f t="shared" si="1"/>
         <v>-47943</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="4">
+        <f t="shared" si="2"/>
+        <v>-5.1047015895561404E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <f>AVERAGE(B2:B11)</f>
+        <v>46031.9</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:M12" si="3">AVERAGE(C2:C11)</f>
+        <v>47330.6</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="3"/>
+        <v>48074.7</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="3"/>
+        <v>58841.7</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="3"/>
+        <v>58252.4</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="3"/>
+        <v>77615.3</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>74659.399999999994</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>86801.600000000006</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="3"/>
+        <v>93421.6</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>69166.5</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="3"/>
+        <v>76175.3</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="3"/>
+        <v>165642.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B12:M12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="7"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
find Lowest average monthly sale and highest average monthly sale
</commit_message>
<xml_diff>
--- a/Discount-Variety-Store-433-Monthly-Sales.xlsx
+++ b/Discount-Variety-Store-433-Monthly-Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\Common-Calculation-Fomulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1347C6F-FEE1-47CD-9F91-7E43E5890C65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3F9607-036E-46B6-99AF-5068C63BA350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Monthly sales</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Average by month</t>
+  </si>
+  <si>
+    <t>Lowest monthly average</t>
+  </si>
+  <si>
+    <t>Highest monthly average</t>
   </si>
 </sst>
 </file>
@@ -354,15 +360,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -993,10 +999,24 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <f>MIN(B12:M12)</f>
+        <v>46031.9</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <f>MAX(B12:M12)</f>
+        <v>165642.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:M12">

</xml_diff>